<commit_message>
update renewcheck with latest files
</commit_message>
<xml_diff>
--- a/renewcheck/run_time_summary.xlsx
+++ b/renewcheck/run_time_summary.xlsx
@@ -483,10 +483,10 @@
         <v>1000</v>
       </c>
       <c r="C2" t="n">
-        <v>12.85562859295169</v>
+        <v>13.90039749804419</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2142604765491948</v>
+        <v>0.2316732916340697</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -495,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1872</v>
+        <v>0.1605</v>
       </c>
     </row>
     <row r="3">
@@ -509,10 +509,10 @@
         <v>1001</v>
       </c>
       <c r="C3" t="n">
-        <v>13.65182987699518</v>
+        <v>10.95645377895562</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2275304979499197</v>
+        <v>0.1826075629825937</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -521,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5025599999999999</v>
+        <v>0.1435</v>
       </c>
     </row>
     <row r="4">
@@ -535,10 +535,10 @@
         <v>1002</v>
       </c>
       <c r="C4" t="n">
-        <v>13.47932489396771</v>
+        <v>13.31739242596086</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2246554148994619</v>
+        <v>0.221956540432681</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -547,10 +547,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6019199999999999</v>
+        <v>0.4735</v>
       </c>
     </row>
     <row r="5">
@@ -561,10 +561,10 @@
         <v>1003</v>
       </c>
       <c r="C5" t="n">
-        <v>12.99607402097899</v>
+        <v>11.88733426597901</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2166012336829833</v>
+        <v>0.1981222377663168</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -573,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H5" t="n">
-        <v>0.24912</v>
+        <v>0.1855</v>
       </c>
     </row>
     <row r="6">
@@ -587,10 +587,10 @@
         <v>1004</v>
       </c>
       <c r="C6" t="n">
-        <v>12.2698243590421</v>
+        <v>14.77310142602073</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2044970726507017</v>
+        <v>0.2462183571003455</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -599,10 +599,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H6" t="n">
-        <v>0.47736</v>
+        <v>0.2165</v>
       </c>
     </row>
     <row r="7">
@@ -613,10 +613,10 @@
         <v>1005</v>
       </c>
       <c r="C7" t="n">
-        <v>12.05136363295605</v>
+        <v>12.01420106296428</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2008560605492676</v>
+        <v>0.2002366843827379</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -625,10 +625,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
-        <v>0.45072</v>
+        <v>0.1785</v>
       </c>
     </row>
     <row r="8">
@@ -639,10 +639,10 @@
         <v>1006</v>
       </c>
       <c r="C8" t="n">
-        <v>13.14844690699829</v>
+        <v>12.3738195389742</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2191407817833048</v>
+        <v>0.2062303256495701</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -651,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H8" t="n">
-        <v>0.20088</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="9">
@@ -665,10 +665,10 @@
         <v>1007</v>
       </c>
       <c r="C9" t="n">
-        <v>12.01246620999882</v>
+        <v>11.8163995060022</v>
       </c>
       <c r="D9" t="n">
-        <v>0.200207770166647</v>
+        <v>0.1969399917667033</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -677,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>0.24336</v>
+        <v>0.194</v>
       </c>
     </row>
     <row r="10">
@@ -691,10 +691,10 @@
         <v>1008</v>
       </c>
       <c r="C10" t="n">
-        <v>12.15883969201241</v>
+        <v>12.72311194601934</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2026473282002068</v>
+        <v>0.2120518657669891</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -703,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>0.19152</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="11">
@@ -717,10 +717,10 @@
         <v>1009</v>
       </c>
       <c r="C11" t="n">
-        <v>13.31405165500473</v>
+        <v>13.56504021596629</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2219008609167455</v>
+        <v>0.2260840035994382</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -729,10 +729,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H11" t="n">
-        <v>0.26712</v>
+        <v>0.3115</v>
       </c>
     </row>
     <row r="12">
@@ -743,10 +743,10 @@
         <v>1010</v>
       </c>
       <c r="C12" t="n">
-        <v>12.53016412799479</v>
+        <v>12.12102032103576</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2088360687999132</v>
+        <v>0.202017005350596</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -755,10 +755,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H12" t="n">
-        <v>0.26712</v>
+        <v>0.1615</v>
       </c>
     </row>
     <row r="13">
@@ -769,10 +769,10 @@
         <v>1011</v>
       </c>
       <c r="C13" t="n">
-        <v>12.92550763196778</v>
+        <v>14.29007622494828</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2154251271994629</v>
+        <v>0.2381679370824713</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -781,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H13" t="n">
-        <v>0.27288</v>
+        <v>0.352</v>
       </c>
     </row>
     <row r="14">
@@ -795,10 +795,10 @@
         <v>1012</v>
       </c>
       <c r="C14" t="n">
-        <v>12.99799261498265</v>
+        <v>12.65575396001805</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2166332102497108</v>
+        <v>0.2109292326669674</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -807,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
-        <v>0.7372799999999999</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="15">
@@ -821,10 +821,10 @@
         <v>1013</v>
       </c>
       <c r="C15" t="n">
-        <v>12.09997530898545</v>
+        <v>12.72773971100105</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2016662551497575</v>
+        <v>0.2121289951833508</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -833,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5011199999999999</v>
+        <v>0.1715</v>
       </c>
     </row>
     <row r="16">
@@ -847,10 +847,10 @@
         <v>1014</v>
       </c>
       <c r="C16" t="n">
-        <v>12.60438484000042</v>
+        <v>14.48529980098829</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2100730806666737</v>
+        <v>0.2414216633498048</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -859,10 +859,10 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="H16" t="n">
-        <v>0.27288</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="17">
@@ -873,10 +873,10 @@
         <v>1015</v>
       </c>
       <c r="C17" t="n">
-        <v>11.38465392199578</v>
+        <v>13.22807990998263</v>
       </c>
       <c r="D17" t="n">
-        <v>0.189744232033263</v>
+        <v>0.2204679984997104</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -885,10 +885,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H17" t="n">
-        <v>0.21096</v>
+        <v>0.289</v>
       </c>
     </row>
     <row r="18">
@@ -899,10 +899,10 @@
         <v>1016</v>
       </c>
       <c r="C18" t="n">
-        <v>11.87774880003417</v>
+        <v>12.42108130198903</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1979624800005695</v>
+        <v>0.2070180216998172</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -914,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="H18" t="n">
-        <v>0.23688</v>
+        <v>0.1545</v>
       </c>
     </row>
     <row r="19">
@@ -925,10 +925,10 @@
         <v>1017</v>
       </c>
       <c r="C19" t="n">
-        <v>11.9683892740286</v>
+        <v>12.0456357980147</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1994731545671433</v>
+        <v>0.2007605966335783</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -937,10 +937,10 @@
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H19" t="n">
-        <v>0.16704</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="20">
@@ -951,10 +951,10 @@
         <v>1018</v>
       </c>
       <c r="C20" t="n">
-        <v>12.46494103601435</v>
+        <v>12.78579435800202</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2077490172669059</v>
+        <v>0.213096572633367</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -963,10 +963,10 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H20" t="n">
-        <v>0.23184</v>
+        <v>0.3575</v>
       </c>
     </row>
     <row r="21">
@@ -977,10 +977,10 @@
         <v>1019</v>
       </c>
       <c r="C21" t="n">
-        <v>12.40690079302294</v>
+        <v>14.2419447050197</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2067816798837157</v>
+        <v>0.2373657450836618</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -989,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4298399999999999</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="22">
@@ -1003,10 +1003,10 @@
         <v>1020</v>
       </c>
       <c r="C22" t="n">
-        <v>13.13104962202488</v>
+        <v>12.07460578397149</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2188508270337479</v>
+        <v>0.2012434297328582</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1015,10 +1015,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H22" t="n">
-        <v>0.23832</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="23">
@@ -1029,10 +1029,10 @@
         <v>1021</v>
       </c>
       <c r="C23" t="n">
-        <v>12.97451749397442</v>
+        <v>12.32046016003005</v>
       </c>
       <c r="D23" t="n">
-        <v>0.216241958232907</v>
+        <v>0.2053410026671675</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1041,10 +1041,10 @@
         <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H23" t="n">
-        <v>0.32184</v>
+        <v>0.1215</v>
       </c>
     </row>
     <row r="24">
@@ -1055,10 +1055,10 @@
         <v>1022</v>
       </c>
       <c r="C24" t="n">
-        <v>12.92803773499327</v>
+        <v>12.63373363803839</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2154672955832211</v>
+        <v>0.2105622273006399</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -1067,10 +1067,10 @@
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" t="n">
-        <v>0.18432</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="25">
@@ -1081,10 +1081,10 @@
         <v>1023</v>
       </c>
       <c r="C25" t="n">
-        <v>12.65122502000304</v>
+        <v>12.77754873700906</v>
       </c>
       <c r="D25" t="n">
-        <v>0.210853750333384</v>
+        <v>0.2129591456168176</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -1093,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25" t="n">
-        <v>0.20952</v>
+        <v>0.166</v>
       </c>
     </row>
     <row r="26">
@@ -1107,10 +1107,10 @@
         <v>1024</v>
       </c>
       <c r="C26" t="n">
-        <v>12.0053770840168</v>
+        <v>12.42840196599718</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2000896180669467</v>
+        <v>0.2071400327666197</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -1119,10 +1119,10 @@
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1692</v>
+        <v>0.1265</v>
       </c>
     </row>
     <row r="27">
@@ -1133,10 +1133,10 @@
         <v>1025</v>
       </c>
       <c r="C27" t="n">
-        <v>12.57973232096992</v>
+        <v>11.30001839197939</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2096622053494987</v>
+        <v>0.1883336398663232</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>0.18648</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="28">
@@ -1159,10 +1159,10 @@
         <v>1026</v>
       </c>
       <c r="C28" t="n">
-        <v>12.86629389703739</v>
+        <v>11.87720039696433</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2144382316172899</v>
+        <v>0.1979533399494054</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -1171,10 +1171,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H28" t="n">
-        <v>0.27864</v>
+        <v>0.141</v>
       </c>
     </row>
     <row r="29">
@@ -1185,10 +1185,10 @@
         <v>1027</v>
       </c>
       <c r="C29" t="n">
-        <v>13.5656726930174</v>
+        <v>12.79001216997858</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2260945448836234</v>
+        <v>0.213166869499643</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -1197,10 +1197,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" t="n">
-        <v>0.26352</v>
+        <v>0.1495</v>
       </c>
     </row>
     <row r="30">
@@ -1211,10 +1211,10 @@
         <v>1028</v>
       </c>
       <c r="C30" t="n">
-        <v>12.45087861997308</v>
+        <v>12.60057264502393</v>
       </c>
       <c r="D30" t="n">
-        <v>0.207514643666218</v>
+        <v>0.2100095440837322</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -1223,10 +1223,10 @@
         <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H30" t="n">
-        <v>0.27792</v>
+        <v>0.1785</v>
       </c>
     </row>
     <row r="31">
@@ -1237,10 +1237,10 @@
         <v>1029</v>
       </c>
       <c r="C31" t="n">
-        <v>12.63535503298044</v>
+        <v>12.43005851196358</v>
       </c>
       <c r="D31" t="n">
-        <v>0.210589250549674</v>
+        <v>0.2071676418660597</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -1249,10 +1249,10 @@
         <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H31" t="n">
-        <v>0.21384</v>
+        <v>0.1225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>